<commit_message>
Update product weights based on modified shipping_rates.xlsx
- Soap weight updated to 95g (from Excel)
- Moringa + Soap: 100g + 95g = 195g (corrected from 200g)
- All other weights verified from Excel Product Grams sheet
</commit_message>
<xml_diff>
--- a/products/shipping/shipping_rates.xlsx
+++ b/products/shipping/shipping_rates.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="283">
   <si>
     <t>Size</t>
   </si>
@@ -824,13 +824,19 @@
     <t>Product Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Variations </t>
+  </si>
+  <si>
     <t>Gram</t>
   </si>
   <si>
     <t>Moringa</t>
   </si>
   <si>
-    <t xml:space="preserve">100g, 200g </t>
+    <t>100g</t>
+  </si>
+  <si>
+    <t>200g</t>
   </si>
   <si>
     <t>Dried Curry Leaves</t>
@@ -842,9 +848,6 @@
     <t xml:space="preserve">Darjeeling Black Tea </t>
   </si>
   <si>
-    <t>100g</t>
-  </si>
-  <si>
     <t>Combo pack</t>
   </si>
   <si>
@@ -854,17 +857,20 @@
     <t xml:space="preserve">Soap </t>
   </si>
   <si>
+    <t>95g</t>
+  </si>
+  <si>
     <t xml:space="preserve">Moringa + Soap </t>
   </si>
   <si>
-    <t xml:space="preserve">200g </t>
+    <t>100g + 95</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -881,6 +887,17 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -911,7 +928,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -922,8 +939,17 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="top"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -11302,7 +11328,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="19.0"/>
     <col customWidth="1" min="2" max="2" width="37.71"/>
-    <col customWidth="1" min="3" max="26" width="8.71"/>
+    <col customWidth="1" min="3" max="3" width="66.86"/>
+    <col customWidth="1" min="4" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -11312,55 +11339,68 @@
       <c r="B1" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="4" t="s">
+        <v>270</v>
+      </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>271</v>
       </c>
+      <c r="B2" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="B5" s="4" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="C6" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>275</v>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="6" t="s">
         <v>280</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>